<commit_message>
Updated with Excel support
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -52,31 +52,37 @@
     <t>pet post api test</t>
   </si>
   <si>
-    <t>http://localhost:8800/api/pets</t>
+    <t>http://mockbin.org/bin/2c5f64fe-4b65-4453-85a5-5308767e79e8</t>
+  </si>
+  <si>
+    <t>application/xml</t>
+  </si>
+  <si>
+    <t>input.xml</t>
+  </si>
+  <si>
+    <t>output.xml</t>
+  </si>
+  <si>
+    <t>VirtualanStdType=EDI-271</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>PetGet</t>
+  </si>
+  <si>
+    <t>get API testing</t>
+  </si>
+  <si>
+    <t>http://localhost:8800/api/pets/findByTags?tags=grey</t>
   </si>
   <si>
     <t>application/json</t>
-  </si>
-  <si>
-    <t>input.json</t>
-  </si>
-  <si>
-    <t>output.json</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>PetGet</t>
-  </si>
-  <si>
-    <t>get API testing</t>
-  </si>
-  <si>
-    <t>http://localhost:8800/api/pets/findByTags?tags=grey</t>
   </si>
   <si>
     <t>get_response.json</t>
@@ -95,22 +101,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
       <color rgb="FF008000"/>
       <name val="Consolas"/>
     </font>
     <font>
-      <color theme="1"/>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FF505050"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <u/>
-      <sz val="9.0"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
+    <font/>
     <font>
       <b/>
       <u/>
@@ -149,11 +155,11 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -385,6 +391,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="2" max="2" width="18.14"/>
     <col customWidth="1" min="3" max="3" width="176.14"/>
     <col customWidth="1" min="6" max="6" width="21.71"/>
     <col customWidth="1" min="8" max="8" width="23.29"/>
@@ -397,31 +404,31 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -432,48 +439,51 @@
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1">
-        <v>201.0</v>
+      <c r="J2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="4">
+        <v>200.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
+      <c r="A3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="3">
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1">
         <v>200.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated with WorkFlow Execution
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -46,56 +46,80 @@
     <t>HttpStatusCode</t>
   </si>
   <si>
+    <t>StoreResponseVariables</t>
+  </si>
+  <si>
+    <t>AddifyVariables</t>
+  </si>
+  <si>
+    <t>EDI-271 API test</t>
+  </si>
+  <si>
+    <t>http://mockbin.org/bin/3f64e65d-c657-42d5-bcc9-5b13e71ca493</t>
+  </si>
+  <si>
+    <t>application/xml</t>
+  </si>
+  <si>
+    <t>input.xml</t>
+  </si>
+  <si>
+    <t>output.xml</t>
+  </si>
+  <si>
+    <t>VirtualanStdType=EDI-271</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>PetGet</t>
+  </si>
+  <si>
+    <t>get API testing</t>
+  </si>
+  <si>
+    <t>https://live.virtualandemo.com/api/pets/findByTags?tags=grey</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>get_response.json</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>petId=id;petName=name</t>
+  </si>
+  <si>
     <t>PetPost</t>
   </si>
   <si>
-    <t>pet post api test</t>
-  </si>
-  <si>
-    <t>http://mockbin.org/bin/2c5f64fe-4b65-4453-85a5-5308767e79e8</t>
-  </si>
-  <si>
-    <t>application/xml</t>
-  </si>
-  <si>
-    <t>input.xml</t>
-  </si>
-  <si>
-    <t>output.xml</t>
-  </si>
-  <si>
-    <t>VirtualanStdType=EDI-271</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>PetGet</t>
-  </si>
-  <si>
-    <t>get API testing</t>
-  </si>
-  <si>
-    <t>https://live.virtualandemo.com/api/pets/findByTags?tags=grey</t>
-  </si>
-  <si>
-    <t>application/json</t>
-  </si>
-  <si>
-    <t>get_response.json</t>
-  </si>
-  <si>
-    <t>GET</t>
+    <t>post API Testing</t>
+  </si>
+  <si>
+    <t>https://live.virtualandemo.com/api/pets</t>
+  </si>
+  <si>
+    <t>post-request.json</t>
+  </si>
+  <si>
+    <t>post-response.json</t>
+  </si>
+  <si>
+    <t>Id=[petId];petName=doggie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -110,13 +134,17 @@
       <color rgb="FF008000"/>
       <name val="Consolas"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <u/>
       <sz val="9.0"/>
       <color rgb="FF505050"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
       <u/>
@@ -145,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -155,13 +183,16 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -395,6 +426,7 @@
     <col customWidth="1" min="3" max="3" width="176.14"/>
     <col customWidth="1" min="6" max="6" width="21.71"/>
     <col customWidth="1" min="8" max="8" width="23.29"/>
+    <col customWidth="1" min="12" max="12" width="21.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -431,60 +463,96 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="4">
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3">
         <v>200.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K3" s="1">
         <v>200.0</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="3">
+        <v>200.0</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -496,7 +564,8 @@
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
     <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="C4"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with WorkFlow Execution with tags
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="API-Testing" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="API-Testing-Sheet2-Duplicate" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -175,6 +176,50 @@
   </si>
   <si>
     <t>Id=[petId];petName=doggie</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Inconsolata"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>tag=</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Inconsolata"/>
+        <b/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>grey</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Inconsolata"/>
+        <b/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>https://live.virtualandemo.com/api/pets/findByTags?tags=</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Inconsolata"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>[tag]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -287,6 +332,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -668,4 +717,190 @@
   </hyperlinks>
   <drawing r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="18.14"/>
+    <col customWidth="1" min="3" max="3" width="176.14"/>
+    <col customWidth="1" min="6" max="6" width="21.71"/>
+    <col customWidth="1" min="8" max="8" width="23.29"/>
+    <col customWidth="1" min="12" max="12" width="49.29"/>
+    <col customWidth="1" min="13" max="13" width="24.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(G3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="M2"/>
+    <hyperlink r:id="rId3" ref="C3"/>
+    <hyperlink r:id="rId4" ref="C4"/>
+  </hyperlinks>
+  <drawing r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>